<commit_message>
adding new excel files
</commit_message>
<xml_diff>
--- a/deaths.xlsx
+++ b/deaths.xlsx
@@ -1,15 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="SimpleXLSXGen"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanl\Desktop\repos\covid-analyzer-py\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E91B8B8-1D03-426E-A791-98DD0E575F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="279">
   <si>
     <t>country</t>
   </si>
@@ -590,9 +601,6 @@
     <t>Norway</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>Luxembourg</t>
   </si>
   <si>
@@ -843,26 +851,31 @@
   </si>
   <si>
     <t>https://www.moph.gov.lb/maps/covid19.php</t>
+  </si>
+  <si>
+    <t>https://malawipublichealth.org/index.php/resources/COVID-19%20Daily%20situation%20Reports/January%202021/Week%201%202021_Malawi%20COVID-19%20weekly%20situation%20report_20210112.pdf/detail</t>
+  </si>
+  <si>
+    <t>Usa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b/>
-    </font>
   </fonts>
-  <fills count="1">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -877,27 +890,329 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F141"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23"/>
     <col min="2" max="2" width="8"/>
@@ -907,7 +1222,7 @@
     <col min="6" max="6" width="60"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -927,7 +1242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -947,7 +1262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -955,7 +1270,7 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>81.82</v>
+        <v>81.819999999999993</v>
       </c>
       <c r="D3">
         <v>18.18</v>
@@ -967,7 +1282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -987,7 +1302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1007,7 +1322,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1015,7 +1330,7 @@
         <v>337</v>
       </c>
       <c r="C6">
-        <v>77.74</v>
+        <v>77.739999999999995</v>
       </c>
       <c r="D6">
         <v>22.26</v>
@@ -1027,7 +1342,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1047,7 +1362,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1063,13 +1378,11 @@
       <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>https://malawipublichealth.org/index.php/resources/COVID-19%20Daily%20situation%20Reports/January%202021/Week%201%202021_Malawi%20COVID-19%20weekly%20situation%20report_20210112.pdf/detail</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
+      <c r="F8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1089,7 +1402,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1109,7 +1422,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1117,7 +1430,7 @@
         <v>6190</v>
       </c>
       <c r="C11">
-        <v>74.15</v>
+        <v>74.150000000000006</v>
       </c>
       <c r="D11">
         <v>25.85</v>
@@ -1129,7 +1442,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1137,7 +1450,7 @@
         <v>56</v>
       </c>
       <c r="C12">
-        <v>71.43</v>
+        <v>71.430000000000007</v>
       </c>
       <c r="D12">
         <v>28.57</v>
@@ -1149,7 +1462,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1166,7 +1479,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1186,7 +1499,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1206,7 +1519,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1214,7 +1527,7 @@
         <v>5892</v>
       </c>
       <c r="C16">
-        <v>69.82</v>
+        <v>69.819999999999993</v>
       </c>
       <c r="D16">
         <v>30.18</v>
@@ -1226,7 +1539,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1234,7 +1547,7 @@
         <v>2070</v>
       </c>
       <c r="C17">
-        <v>69.32</v>
+        <v>69.319999999999993</v>
       </c>
       <c r="D17">
         <v>30.68</v>
@@ -1246,7 +1559,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1266,7 +1579,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1274,7 +1587,7 @@
         <v>1380</v>
       </c>
       <c r="C19">
-        <v>68.99</v>
+        <v>68.989999999999995</v>
       </c>
       <c r="D19">
         <v>31.01</v>
@@ -1283,7 +1596,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -1291,7 +1604,7 @@
         <v>102</v>
       </c>
       <c r="C20">
-        <v>67.65</v>
+        <v>67.650000000000006</v>
       </c>
       <c r="D20">
         <v>32.35</v>
@@ -1303,7 +1616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -1311,7 +1624,7 @@
         <v>113</v>
       </c>
       <c r="C21">
-        <v>67.26</v>
+        <v>67.260000000000005</v>
       </c>
       <c r="D21">
         <v>32.74</v>
@@ -1323,7 +1636,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1331,7 +1644,7 @@
         <v>2077</v>
       </c>
       <c r="C22">
-        <v>66.15</v>
+        <v>66.150000000000006</v>
       </c>
       <c r="D22">
         <v>33.85</v>
@@ -1343,7 +1656,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -1351,7 +1664,7 @@
         <v>5310</v>
       </c>
       <c r="C23">
-        <v>66.01</v>
+        <v>66.010000000000005</v>
       </c>
       <c r="D23">
         <v>33.99</v>
@@ -1363,7 +1676,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -1374,7 +1687,7 @@
         <v>65.88</v>
       </c>
       <c r="D24">
-        <v>34.12</v>
+        <v>34.119999999999997</v>
       </c>
       <c r="E24" t="s">
         <v>66</v>
@@ -1383,7 +1696,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -1391,7 +1704,7 @@
         <v>148</v>
       </c>
       <c r="C25">
-        <v>65.54</v>
+        <v>65.540000000000006</v>
       </c>
       <c r="D25">
         <v>34.46</v>
@@ -1403,7 +1716,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -1423,7 +1736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -1431,7 +1744,7 @@
         <v>3949</v>
       </c>
       <c r="C27">
-        <v>65.18</v>
+        <v>65.180000000000007</v>
       </c>
       <c r="D27">
         <v>34.82</v>
@@ -1443,7 +1756,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -1454,7 +1767,7 @@
         <v>64.98</v>
       </c>
       <c r="D28">
-        <v>35.02</v>
+        <v>35.020000000000003</v>
       </c>
       <c r="E28" t="s">
         <v>77</v>
@@ -1463,7 +1776,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -1480,7 +1793,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -1500,7 +1813,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -1511,13 +1824,13 @@
         <v>64.7</v>
       </c>
       <c r="D31">
-        <v>35.3</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="E31" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -1537,7 +1850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -1557,7 +1870,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -1577,7 +1890,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -1588,7 +1901,7 @@
         <v>63.38</v>
       </c>
       <c r="D35">
-        <v>36.62</v>
+        <v>36.619999999999997</v>
       </c>
       <c r="E35" t="s">
         <v>81</v>
@@ -1597,7 +1910,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -1608,7 +1921,7 @@
         <v>62.59</v>
       </c>
       <c r="D36">
-        <v>37.41</v>
+        <v>37.409999999999997</v>
       </c>
       <c r="E36" t="s">
         <v>7</v>
@@ -1617,7 +1930,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -1637,7 +1950,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -1648,7 +1961,7 @@
         <v>62.05</v>
       </c>
       <c r="D38">
-        <v>37.95</v>
+        <v>37.950000000000003</v>
       </c>
       <c r="E38" t="s">
         <v>36</v>
@@ -1657,7 +1970,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -1677,7 +1990,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -1697,7 +2010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>104</v>
       </c>
@@ -1717,7 +2030,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -1728,7 +2041,7 @@
         <v>61.66</v>
       </c>
       <c r="D42">
-        <v>38.34</v>
+        <v>38.340000000000003</v>
       </c>
       <c r="E42" t="s">
         <v>106</v>
@@ -1737,7 +2050,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>108</v>
       </c>
@@ -1754,7 +2067,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>110</v>
       </c>
@@ -1765,7 +2078,7 @@
         <v>61.52</v>
       </c>
       <c r="D44">
-        <v>38.48</v>
+        <v>38.479999999999997</v>
       </c>
       <c r="E44" t="s">
         <v>36</v>
@@ -1774,7 +2087,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>111</v>
       </c>
@@ -1794,7 +2107,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>114</v>
       </c>
@@ -1811,7 +2124,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>116</v>
       </c>
@@ -1822,13 +2135,13 @@
         <v>60.77</v>
       </c>
       <c r="D47">
-        <v>39.23</v>
+        <v>39.229999999999997</v>
       </c>
       <c r="E47" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>118</v>
       </c>
@@ -1839,7 +2152,7 @@
         <v>60.77</v>
       </c>
       <c r="D48">
-        <v>39.23</v>
+        <v>39.229999999999997</v>
       </c>
       <c r="E48" t="s">
         <v>119</v>
@@ -1848,7 +2161,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>120</v>
       </c>
@@ -1868,7 +2181,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>122</v>
       </c>
@@ -1879,13 +2192,13 @@
         <v>60.66</v>
       </c>
       <c r="D50">
-        <v>39.34</v>
+        <v>39.340000000000003</v>
       </c>
       <c r="E50" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>124</v>
       </c>
@@ -1905,7 +2218,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>127</v>
       </c>
@@ -1916,7 +2229,7 @@
         <v>60.09</v>
       </c>
       <c r="D52">
-        <v>39.91</v>
+        <v>39.909999999999997</v>
       </c>
       <c r="E52" t="s">
         <v>128</v>
@@ -1925,7 +2238,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>129</v>
       </c>
@@ -1945,7 +2258,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>130</v>
       </c>
@@ -1965,7 +2278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>131</v>
       </c>
@@ -1976,13 +2289,13 @@
         <v>59.59</v>
       </c>
       <c r="D55">
-        <v>40.41</v>
+        <v>40.409999999999997</v>
       </c>
       <c r="E55" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>133</v>
       </c>
@@ -1999,7 +2312,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>135</v>
       </c>
@@ -2019,7 +2332,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>136</v>
       </c>
@@ -2036,7 +2349,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>137</v>
       </c>
@@ -2056,7 +2369,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>139</v>
       </c>
@@ -2076,7 +2389,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>142</v>
       </c>
@@ -2096,7 +2409,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>145</v>
       </c>
@@ -2116,7 +2429,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>147</v>
       </c>
@@ -2136,7 +2449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>148</v>
       </c>
@@ -2156,7 +2469,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>150</v>
       </c>
@@ -2176,7 +2489,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>152</v>
       </c>
@@ -2193,7 +2506,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>154</v>
       </c>
@@ -2213,7 +2526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>156</v>
       </c>
@@ -2233,7 +2546,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>158</v>
       </c>
@@ -2253,7 +2566,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>161</v>
       </c>
@@ -2273,7 +2586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>162</v>
       </c>
@@ -2293,7 +2606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>163</v>
       </c>
@@ -2313,7 +2626,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>165</v>
       </c>
@@ -2333,7 +2646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>166</v>
       </c>
@@ -2353,7 +2666,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>169</v>
       </c>
@@ -2373,7 +2686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>170</v>
       </c>
@@ -2393,7 +2706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>171</v>
       </c>
@@ -2413,7 +2726,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>174</v>
       </c>
@@ -2433,7 +2746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>175</v>
       </c>
@@ -2453,7 +2766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>176</v>
       </c>
@@ -2473,7 +2786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>177</v>
       </c>
@@ -2490,7 +2803,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>179</v>
       </c>
@@ -2510,7 +2823,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>180</v>
       </c>
@@ -2530,7 +2843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>181</v>
       </c>
@@ -2550,7 +2863,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>183</v>
       </c>
@@ -2570,7 +2883,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>184</v>
       </c>
@@ -2590,7 +2903,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>186</v>
       </c>
@@ -2610,7 +2923,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>187</v>
       </c>
@@ -2630,7 +2943,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>190</v>
       </c>
@@ -2650,7 +2963,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>191</v>
       </c>
@@ -2670,7 +2983,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>192</v>
       </c>
@@ -2690,9 +3003,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>193</v>
+        <v>278</v>
       </c>
       <c r="B92">
         <v>845385</v>
@@ -2707,9 +3020,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B93">
         <v>1082</v>
@@ -2721,15 +3034,15 @@
         <v>45.01</v>
       </c>
       <c r="E93" t="s">
+        <v>194</v>
+      </c>
+      <c r="F93" t="s">
         <v>195</v>
       </c>
-      <c r="F93" t="s">
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>197</v>
       </c>
       <c r="B94">
         <v>34849</v>
@@ -2741,15 +3054,15 @@
         <v>45.07</v>
       </c>
       <c r="E94" t="s">
+        <v>197</v>
+      </c>
+      <c r="F94" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>198</v>
-      </c>
-      <c r="F94" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
-        <v>199</v>
       </c>
       <c r="B95">
         <v>6417</v>
@@ -2761,15 +3074,15 @@
         <v>45.32</v>
       </c>
       <c r="E95" t="s">
+        <v>199</v>
+      </c>
+      <c r="F95" t="s">
         <v>200</v>
       </c>
-      <c r="F95" t="s">
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>202</v>
       </c>
       <c r="B96">
         <v>22769</v>
@@ -2787,9 +3100,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B97">
         <v>132906</v>
@@ -2807,9 +3120,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B98">
         <v>65788</v>
@@ -2827,9 +3140,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B99">
         <v>3444</v>
@@ -2841,15 +3154,15 @@
         <v>45.41</v>
       </c>
       <c r="E99" t="s">
+        <v>205</v>
+      </c>
+      <c r="F99" t="s">
         <v>206</v>
       </c>
-      <c r="F99" t="s">
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s">
-        <v>208</v>
       </c>
       <c r="B100">
         <v>370</v>
@@ -2867,9 +3180,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B101">
         <v>2085</v>
@@ -2881,15 +3194,15 @@
         <v>45.71</v>
       </c>
       <c r="E101" t="s">
+        <v>209</v>
+      </c>
+      <c r="F101" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>210</v>
-      </c>
-      <c r="F101" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s">
-        <v>211</v>
       </c>
       <c r="B102">
         <v>10183</v>
@@ -2904,12 +3217,12 @@
         <v>188</v>
       </c>
       <c r="F102" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s">
-        <v>213</v>
       </c>
       <c r="B103">
         <v>3170</v>
@@ -2927,9 +3240,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B104">
         <v>27296</v>
@@ -2947,9 +3260,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B105">
         <v>4849</v>
@@ -2967,9 +3280,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B106">
         <v>6799</v>
@@ -2981,15 +3294,15 @@
         <v>46.36</v>
       </c>
       <c r="E106" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F106" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B107">
         <v>31542</v>
@@ -3007,9 +3320,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B108">
         <v>1462</v>
@@ -3021,15 +3334,15 @@
         <v>46.92</v>
       </c>
       <c r="E108" t="s">
+        <v>219</v>
+      </c>
+      <c r="F108" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>220</v>
-      </c>
-      <c r="F108" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s">
-        <v>221</v>
       </c>
       <c r="B109">
         <v>12901</v>
@@ -3041,12 +3354,12 @@
         <v>47</v>
       </c>
       <c r="E109" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="s">
-        <v>223</v>
       </c>
       <c r="B110">
         <v>202862</v>
@@ -3064,9 +3377,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B111">
         <v>1294</v>
@@ -3081,12 +3394,12 @@
         <v>188</v>
       </c>
       <c r="F111" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="s">
-        <v>226</v>
       </c>
       <c r="B112">
         <v>91056</v>
@@ -3104,9 +3417,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B113">
         <v>49836</v>
@@ -3124,9 +3437,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B114">
         <v>147613</v>
@@ -3138,15 +3451,15 @@
         <v>47.81</v>
       </c>
       <c r="E114" t="s">
+        <v>228</v>
+      </c>
+      <c r="F114" t="s">
         <v>229</v>
       </c>
-      <c r="F114" t="s">
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="s">
-        <v>231</v>
       </c>
       <c r="B115">
         <v>64052</v>
@@ -3164,9 +3477,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B116">
         <v>37982</v>
@@ -3184,9 +3497,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B117">
         <v>14858</v>
@@ -3198,15 +3511,15 @@
         <v>48.18</v>
       </c>
       <c r="E117" t="s">
+        <v>233</v>
+      </c>
+      <c r="F117" t="s">
         <v>234</v>
       </c>
-      <c r="F117" t="s">
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="s">
-        <v>236</v>
       </c>
       <c r="B118">
         <v>671</v>
@@ -3221,12 +3534,12 @@
         <v>10</v>
       </c>
       <c r="F118" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="s">
-        <v>238</v>
       </c>
       <c r="B119">
         <v>2853</v>
@@ -3238,15 +3551,15 @@
         <v>48.44</v>
       </c>
       <c r="E119" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F119" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B120">
         <v>12696</v>
@@ -3264,9 +3577,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B121">
         <v>83540</v>
@@ -3284,9 +3597,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B122">
         <v>16366</v>
@@ -3304,9 +3617,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B123">
         <v>1007</v>
@@ -3318,15 +3631,15 @@
         <v>50.25</v>
       </c>
       <c r="E123" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F123" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B124">
         <v>5092</v>
@@ -3344,9 +3657,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B125">
         <v>53</v>
@@ -3358,15 +3671,15 @@
         <v>50.94</v>
       </c>
       <c r="E125" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F125" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B126">
         <v>24399</v>
@@ -3381,12 +3694,12 @@
         <v>188</v>
       </c>
       <c r="F126" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="s">
-        <v>249</v>
       </c>
       <c r="B127">
         <v>103512</v>
@@ -3401,12 +3714,12 @@
         <v>81</v>
       </c>
       <c r="F127" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="s">
-        <v>251</v>
       </c>
       <c r="B128">
         <v>21</v>
@@ -3421,12 +3734,12 @@
         <v>117</v>
       </c>
       <c r="F128" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="s">
-        <v>253</v>
       </c>
       <c r="B129">
         <v>286</v>
@@ -3438,15 +3751,15 @@
         <v>52.45</v>
       </c>
       <c r="E129" t="s">
+        <v>253</v>
+      </c>
+      <c r="F129" t="s">
         <v>254</v>
       </c>
-      <c r="F129" t="s">
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="s">
-        <v>256</v>
       </c>
       <c r="B130">
         <v>15176</v>
@@ -3464,9 +3777,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B131">
         <v>18530</v>
@@ -3484,9 +3797,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B132">
         <v>11364</v>
@@ -3504,9 +3817,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B133">
         <v>205917</v>
@@ -3524,9 +3837,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B134">
         <v>37</v>
@@ -3538,15 +3851,15 @@
         <v>54.05</v>
       </c>
       <c r="E134" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F134" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B135">
         <v>2183</v>
@@ -3564,9 +3877,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B136">
         <v>73</v>
@@ -3584,9 +3897,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B137">
         <v>86</v>
@@ -3598,15 +3911,15 @@
         <v>56.98</v>
       </c>
       <c r="E137" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F137" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="s">
-        <v>266</v>
       </c>
       <c r="B138">
         <v>7</v>
@@ -3618,15 +3931,15 @@
         <v>57.14</v>
       </c>
       <c r="E138" t="s">
+        <v>266</v>
+      </c>
+      <c r="F138" t="s">
         <v>267</v>
       </c>
-      <c r="F138" t="s">
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="s">
-        <v>269</v>
       </c>
       <c r="B139">
         <v>15</v>
@@ -3638,15 +3951,15 @@
         <v>60</v>
       </c>
       <c r="E139" t="s">
+        <v>269</v>
+      </c>
+      <c r="F139" t="s">
         <v>270</v>
       </c>
-      <c r="F139" t="s">
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="s">
-        <v>272</v>
       </c>
       <c r="B140">
         <v>13</v>
@@ -3658,15 +3971,15 @@
         <v>61.54</v>
       </c>
       <c r="E140" t="s">
+        <v>272</v>
+      </c>
+      <c r="F140" t="s">
         <v>273</v>
       </c>
-      <c r="F140" t="s">
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="s">
-        <v>275</v>
       </c>
       <c r="B141">
         <v>36</v>
@@ -3678,12 +3991,13 @@
         <v>69.44</v>
       </c>
       <c r="E141" t="s">
+        <v>275</v>
+      </c>
+      <c r="F141" t="s">
         <v>276</v>
       </c>
-      <c r="F141" t="s">
-        <v>277</v>
-      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>